<commit_message>
Esclarecendo os processos do Gráfico Bolha da Avaliação
</commit_message>
<xml_diff>
--- a/Documentos Gerados/Fase 1/GráficoBolhaDaAvaliaçãoDosProcessos.xlsx
+++ b/Documentos Gerados/Fase 1/GráficoBolhaDaAvaliaçãoDosProcessos.xlsx
@@ -70,10 +70,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="132"/>
+      <c14:style val="148"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="32"/>
+      <c:style val="48"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -84,120 +84,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr>
-                <a:solidFill>
-                  <a:schemeClr val="dk1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pt-BR" b="1" cap="all" spc="0">
-                <a:ln w="9000" cmpd="sng">
-                  <a:solidFill>
-                    <a:schemeClr val="accent4">
-                      <a:shade val="50000"/>
-                      <a:satMod val="120000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:prstDash val="solid"/>
-                </a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="dk1"/>
-                </a:solidFill>
-                <a:effectLst>
-                  <a:reflection blurRad="12700" stA="28000" endPos="45000" dist="1000" dir="5400000" sy="-100000" algn="bl" rotWithShape="0"/>
-                </a:effectLst>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:rPr>
-              <a:t>Avaliação</a:t>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Avaliação dos Processos</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR" b="1" cap="all" spc="0" baseline="0">
-                <a:ln w="9000" cmpd="sng">
-                  <a:solidFill>
-                    <a:schemeClr val="accent4">
-                      <a:shade val="50000"/>
-                      <a:satMod val="120000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:prstDash val="solid"/>
-                </a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="dk1"/>
-                </a:solidFill>
-                <a:effectLst>
-                  <a:reflection blurRad="12700" stA="28000" endPos="45000" dist="1000" dir="5400000" sy="-100000" algn="bl" rotWithShape="0"/>
-                </a:effectLst>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:rPr>
-              <a:t> dos Processos</a:t>
-            </a:r>
-            <a:endParaRPr lang="pt-BR" b="1" cap="all" spc="0">
-              <a:ln w="9000" cmpd="sng">
-                <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:shade val="50000"/>
-                    <a:satMod val="120000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent4">
-                      <a:shade val="20000"/>
-                      <a:satMod val="245000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="43000">
-                    <a:schemeClr val="accent4">
-                      <a:satMod val="255000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="48000">
-                    <a:schemeClr val="accent4">
-                      <a:shade val="85000"/>
-                      <a:satMod val="255000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent4">
-                      <a:shade val="20000"/>
-                      <a:satMod val="245000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000"/>
-              </a:gradFill>
-              <a:effectLst>
-                <a:reflection blurRad="12700" stA="28000" endPos="45000" dist="1000" dir="5400000" sy="-100000" algn="bl" rotWithShape="0"/>
-              </a:effectLst>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -246,11 +143,6 @@
           <c:tx>
             <c:v>Processo de Montagem</c:v>
           </c:tx>
-          <c:spPr>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:xVal>
             <c:numLit>
@@ -287,11 +179,6 @@
           <c:tx>
             <c:v>Processo de Instalação</c:v>
           </c:tx>
-          <c:spPr>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:xVal>
             <c:numLit>
@@ -328,11 +215,6 @@
           <c:tx>
             <c:v>Processo de Estoque</c:v>
           </c:tx>
-          <c:spPr>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:xVal>
             <c:numLit>
@@ -369,11 +251,6 @@
           <c:tx>
             <c:v>Processo de RH</c:v>
           </c:tx>
-          <c:spPr>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:xVal>
             <c:numLit>
@@ -410,11 +287,6 @@
           <c:tx>
             <c:v>Processo de Tercerização</c:v>
           </c:tx>
-          <c:spPr>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:xVal>
             <c:numLit>
@@ -455,11 +327,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="43865600"/>
-        <c:axId val="43867520"/>
+        <c:axId val="44848640"/>
+        <c:axId val="44850560"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="43865600"/>
+        <c:axId val="44848640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -467,13 +339,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:prstDash val="dashDot"/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -497,25 +363,19 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43867520"/>
+        <c:crossAx val="44850560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43867520"/>
+        <c:axId val="44850560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln cmpd="thinThick">
-              <a:prstDash val="dashDot"/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -527,13 +387,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR"/>
-                  <a:t>Importância</a:t>
+                  <a:t>Importância do Processo</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="pt-BR" baseline="0"/>
-                  <a:t> do Processo</a:t>
-                </a:r>
-                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -544,7 +399,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43865600"/>
+        <c:crossAx val="44848640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -618,8 +473,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
-          <a:off x="595313" y="3160568"/>
-          <a:ext cx="8853921" cy="10824"/>
+          <a:off x="595320" y="3154912"/>
+          <a:ext cx="8853917" cy="10772"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -915,6 +770,504 @@
               </a:solidFill>
             </a:rPr>
             <a:t>Alto</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.64686</cdr:x>
+      <cdr:y>0.19604</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.75897</cdr:x>
+      <cdr:y>0.2446</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="CaixaDeTexto 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6245369" y="1179801"/>
+          <a:ext cx="1082387" cy="292244"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.64013</cdr:x>
+      <cdr:y>0.19964</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.78139</cdr:x>
+      <cdr:y>0.27878</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="CaixaDeTexto 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6180426" y="1201450"/>
+          <a:ext cx="1363807" cy="476249"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Processo de Venda</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.56951</cdr:x>
+      <cdr:y>0.36871</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.67489</cdr:x>
+      <cdr:y>0.45683</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="CaixaDeTexto 3"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5498522" y="2218892"/>
+          <a:ext cx="1017443" cy="530370"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Processo  de Montagem</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.38531</cdr:x>
+      <cdr:y>0.37175</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.49069</cdr:x>
+      <cdr:y>0.45988</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="13" name="CaixaDeTexto 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3720091" y="2237221"/>
+          <a:ext cx="1017443" cy="530370"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Processo de Estoque</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.38419</cdr:x>
+      <cdr:y>0.557</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.48957</cdr:x>
+      <cdr:y>0.64513</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="17" name="CaixaDeTexto 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3709265" y="3352079"/>
+          <a:ext cx="1017443" cy="530370"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Processo de Instalação</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.30045</cdr:x>
+      <cdr:y>0.48686</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.3935</cdr:x>
+      <cdr:y>0.58813</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="21" name="CaixaDeTexto 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2900796" y="2929947"/>
+          <a:ext cx="898380" cy="609455"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Processo    de RH</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.19921</cdr:x>
+      <cdr:y>0.62355</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.30459</cdr:x>
+      <cdr:y>0.71168</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="22" name="CaixaDeTexto 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1923328" y="3752561"/>
+          <a:ext cx="1017443" cy="530370"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Processo de Tercerização</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>

</xml_diff>

<commit_message>
Corrigido erro no gráfico bolha
</commit_message>
<xml_diff>
--- a/Documentos Gerados/Fase 1/GráficoBolhaDaAvaliaçãoDosProcessos.xlsx
+++ b/Documentos Gerados/Fase 1/GráficoBolhaDaAvaliaçãoDosProcessos.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="8505"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="19440" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="Gráf1" sheetId="4" r:id="rId1"/>
@@ -141,7 +141,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Processo de Montagem</c:v>
+            <c:v>Processo de Instalação</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:xVal>
@@ -177,7 +177,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Processo de Instalação</c:v>
+            <c:v>Processo de Manutenção</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:xVal>
@@ -327,11 +327,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="44848640"/>
-        <c:axId val="44850560"/>
+        <c:axId val="70174400"/>
+        <c:axId val="70174976"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="44848640"/>
+        <c:axId val="70174400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -363,12 +363,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44850560"/>
+        <c:crossAx val="70174976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44850560"/>
+        <c:axId val="70174976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -399,7 +399,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44848640"/>
+        <c:crossAx val="70174400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -421,7 +421,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -432,7 +432,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9654886" cy="6018068"/>
+    <xdr:ext cx="9637661" cy="6001774"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1"/>
@@ -871,7 +871,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="pt-BR" sz="1100"/>
-            <a:t>Processo  de Montagem</a:t>
+            <a:t>Processo  de Instalação</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -1069,7 +1069,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="pt-BR" sz="1100"/>
-            <a:t>Processo de Instalação</a:t>
+            <a:t>Processo de Manutenção</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>

</xml_diff>